<commit_message>
Updated to show Weight as required attribute
</commit_message>
<xml_diff>
--- a/Draft Schema/Draft Weights and Condition Scores.xlsx
+++ b/Draft Schema/Draft Weights and Condition Scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagaraja\Dropbox (Rezare Systems)\RezareProjects\MLA\ISC Animal Schema\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17B6C63-224F-489E-BDD6-A8B96250CADB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63CB908-7D4C-4E2D-93D9-14D145E7FA3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="749" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="749" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="icarEventCoreResource" sheetId="14" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="94">
   <si>
     <t>Entity</t>
   </si>
@@ -345,6 +345,9 @@
   </si>
   <si>
     <t>iscEventCoreResource</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -1404,8 +1407,8 @@
   </sheetPr>
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,6 +1506,9 @@
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>39</v>
@@ -2285,8 +2291,8 @@
   </sheetPr>
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrected camel case typo for traitLabel
</commit_message>
<xml_diff>
--- a/Draft Schema/Draft Weights and Condition Scores.xlsx
+++ b/Draft Schema/Draft Weights and Condition Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagaraja\Dropbox (Rezare Systems)\RezareProjects\MLA\ISC Animal Schema\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63CB908-7D4C-4E2D-93D9-14D145E7FA3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9D7217-0645-4FB8-B99A-E2FE3B19CCB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="749" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,9 +157,6 @@
     <t>device</t>
   </si>
   <si>
-    <t>traitlabel</t>
-  </si>
-  <si>
     <t>56, (minimum 0)</t>
   </si>
   <si>
@@ -259,9 +256,6 @@
   </si>
   <si>
     <t>2.1, 3.2</t>
-  </si>
-  <si>
-    <t>Usually measured in Millimeters</t>
   </si>
   <si>
     <t>Range applicable for the score value</t>
@@ -348,6 +342,12 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Usually measured in Millimeters. Applicable for Fat Score</t>
+  </si>
+  <si>
+    <t>traitLabel</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1003,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,7 +1021,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B8" s="40" t="s">
         <v>11</v>
@@ -1408,7 +1408,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,10 +1487,10 @@
         <v>31</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="55"/>
@@ -1508,13 +1508,13 @@
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1522,13 +1522,13 @@
         <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -1536,13 +1536,13 @@
         <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1553,7 +1553,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1561,35 +1561,35 @@
         <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1896,7 +1896,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="54"/>
       <c r="C6" s="54"/>
@@ -1965,45 +1965,45 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2292,7 +2292,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,7 +2310,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -2368,13 +2368,13 @@
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="55"/>
@@ -2386,100 +2386,100 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="58" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated with Webinar discussion points
1.	Specified default for ‘units’ as KGM
2.	Added enum ‘Unspecified’ for ‘method’
3.	‘timeOffFeed’ and ‘weight’  specified as double
4.	Split the score object into different objects for Fat, Muscle, Condition and Frame scoring. Score object now has a reference to a scheme for identifying the scoring attributes. Hence would not need a scoreType attribute.
</commit_message>
<xml_diff>
--- a/Draft Schema/Draft Weights and Condition Scores.xlsx
+++ b/Draft Schema/Draft Weights and Condition Scores.xlsx
@@ -8,20 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagaraja\Dropbox (Rezare Systems)\RezareProjects\MLA\ISC Animal Schema\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046E708D-5AF2-47C4-A44C-B7DF99C883E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EDD229-7B8C-47CA-BACC-64F80D4B7D35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="749" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="icarEventCoreResource" sheetId="14" r:id="rId1"/>
     <sheet name="iscWeightEventResource" sheetId="24" r:id="rId2"/>
     <sheet name="iscDeviceReferenceType" sheetId="25" r:id="rId3"/>
-    <sheet name="iscScoreEventCore" sheetId="33" r:id="rId4"/>
+    <sheet name="iscScoreEventCore" sheetId="34" r:id="rId4"/>
+    <sheet name="iscFatScore" sheetId="33" r:id="rId5"/>
+    <sheet name="iscFrameScore" sheetId="37" r:id="rId6"/>
+    <sheet name="iscMuscleScore" sheetId="36" r:id="rId7"/>
+    <sheet name="iscConditionScore" sheetId="35" r:id="rId8"/>
+    <sheet name="iscScoreReference" sheetId="38" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">icarEventCoreResource!$A$1:$G$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">iscConditionScore!$A$1:$G$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">iscDeviceReferenceType!$A$1:$G$38</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">iscScoreEventCore!$A$1:$G$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">iscFatScore!$A$1:$G$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">iscFrameScore!$A$1:$G$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">iscMuscleScore!$A$1:$G$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">iscScoreEventCore!$A$1:$G$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">iscScoreReference!$A$1:$G$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">iscWeightEventResource!$A$1:$G$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -40,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="121">
   <si>
     <t>Entity</t>
   </si>
@@ -94,9 +104,6 @@
   </si>
   <si>
     <t>https://github.com/adewg/ICAR/blob/master/Release%20Candidate%20Messages/icarAnimalIdentifierType.json</t>
-  </si>
-  <si>
-    <t>number</t>
   </si>
   <si>
     <t>id</t>
@@ -219,52 +226,22 @@
     <t>Optionally, the serial number of the device.</t>
   </si>
   <si>
-    <t>scoreType</t>
-  </si>
-  <si>
-    <t>Enumeration - frame, condition, muscle</t>
-  </si>
-  <si>
-    <t>1-12, 1-8, A-E</t>
-  </si>
-  <si>
     <t>https://github.com/adewg/ICAR/blob/master/Release%20Candidate%20Messages/icarResourceReferenceType.json</t>
   </si>
   <si>
     <t>ICAR</t>
   </si>
   <si>
-    <t>1, 2, 2.5, 12, A, C, E</t>
-  </si>
-  <si>
-    <t>Enum - High to Low , Low to High</t>
-  </si>
-  <si>
     <t>Joe Bloggs</t>
   </si>
   <si>
     <t>Name of the assessor</t>
   </si>
   <si>
-    <t>float</t>
-  </si>
-  <si>
     <t>P8, 12th rib</t>
   </si>
   <si>
     <t>2.1, 3.2</t>
-  </si>
-  <si>
-    <t>Range applicable for the score value</t>
-  </si>
-  <si>
-    <t>Order in which the score value should be read and comprehended</t>
-  </si>
-  <si>
-    <t>The type of score being assessed.</t>
-  </si>
-  <si>
-    <t>Value of the score being assessed</t>
   </si>
   <si>
     <t>score</t>
@@ -310,16 +287,7 @@
     <t>Body Site where the measurement was taken. Applicable for Fat Score</t>
   </si>
   <si>
-    <t>measurement</t>
-  </si>
-  <si>
     <t>bodySite</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
-    <t>order</t>
   </si>
   <si>
     <t>assessor</t>
@@ -348,13 +316,140 @@
   <si>
     <t>iscScoreEventCore
 inherits allOf icarEventCoreResource</t>
+  </si>
+  <si>
+    <t>Y, default KGM</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>iscFatScore</t>
+  </si>
+  <si>
+    <t>iscConditionScore</t>
+  </si>
+  <si>
+    <t>iscFrameScore</t>
+  </si>
+  <si>
+    <t>iscMuscleScore</t>
+  </si>
+  <si>
+    <t>iscFatScore
+inherits allOf iscScoreEventCore</t>
+  </si>
+  <si>
+    <t>fatDepth</t>
+  </si>
+  <si>
+    <t>fatDepths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">array of boy sites and fat depth values </t>
+  </si>
+  <si>
+    <t>iscScoreReference</t>
+  </si>
+  <si>
+    <t>fatScoreReference</t>
+  </si>
+  <si>
+    <t>iscFrameScore
+inherits allOf iscScoreEventCore</t>
+  </si>
+  <si>
+    <t>frameScoreReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3, 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value of the fat score </t>
+  </si>
+  <si>
+    <t>iscMuscleScore
+inherits allOf iscScoreEventCore</t>
+  </si>
+  <si>
+    <t>muscleScoreReference</t>
+  </si>
+  <si>
+    <t>A, B, C, D, E</t>
+  </si>
+  <si>
+    <t>iscConditionScore
+inherits allOf iscScoreEventCore</t>
+  </si>
+  <si>
+    <t>conditionScoreReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, 2 </t>
+  </si>
+  <si>
+    <t>sting</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>referenceURL</t>
+  </si>
+  <si>
+    <t>nsw-beefcattle</t>
+  </si>
+  <si>
+    <t>https://www.dpi.nsw.gov.au/animals-and-livestock/beef-cattle/appraisal/publications/frame-scoring</t>
+  </si>
+  <si>
+    <t>Version reference of the particular scheme being followed for scoring</t>
+  </si>
+  <si>
+    <t>The scheme or scoring reference guideline being used</t>
+  </si>
+  <si>
+    <t>Ready links to documentation about the scoring scheme or reference being used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value of the muscle score . Muscle score measures the degree of muscularity of an animal and describes the shape of cattle independent of the influence of fatness. </t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>Event object for capturing Fat Score details</t>
+  </si>
+  <si>
+    <t>Event object for capturing Condition Score details</t>
+  </si>
+  <si>
+    <t>Event object for capturing Frame Score details</t>
+  </si>
+  <si>
+    <t>Event object for capturing Muscle Score details</t>
+  </si>
+  <si>
+    <t>Species for which the scoring scheme applies to</t>
+  </si>
+  <si>
+    <t>Country to which the scoring scheme appies to</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Value of the frame score. Frame score is a  convenient way to discuss and evaluate height is in units of 'frame score' based on the height over the hips at a given age</t>
+  </si>
+  <si>
+    <t>Value of the condition score . Body condition scoring is a visual assessment of the amount of fat and muscle covering the bones of a cow, regardless of body size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,6 +555,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -503,7 +605,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -651,6 +753,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1002,8 +1113,8 @@
   </sheetPr>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,7 +1132,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -1085,7 +1196,7 @@
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B8" s="40" t="s">
         <v>11</v>
@@ -1105,7 +1216,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="39"/>
       <c r="B9" s="40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>7</v>
@@ -1113,14 +1224,14 @@
       <c r="D9" s="41"/>
       <c r="E9" s="42"/>
       <c r="F9" s="43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="36"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="39"/>
       <c r="B10" s="40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="44" t="s">
         <v>14</v>
@@ -1137,7 +1248,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="39"/>
       <c r="B11" s="53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="44" t="s">
         <v>7</v>
@@ -1145,14 +1256,14 @@
       <c r="D11" s="41"/>
       <c r="E11" s="42"/>
       <c r="F11" s="37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G11" s="36"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="39"/>
       <c r="B12" s="53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="44" t="s">
         <v>7</v>
@@ -1160,14 +1271,14 @@
       <c r="D12" s="41"/>
       <c r="E12" s="42"/>
       <c r="F12" s="37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G12" s="36"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="39"/>
       <c r="B13" s="44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="40" t="s">
         <v>15</v>
@@ -1175,21 +1286,21 @@
       <c r="D13" s="41"/>
       <c r="E13" s="42"/>
       <c r="F13" s="45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="39"/>
       <c r="B14" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="40" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>28</v>
       </c>
       <c r="D14" s="41"/>
       <c r="E14" s="42"/>
       <c r="F14" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -1408,7 +1519,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,7 +1537,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -1484,112 +1595,115 @@
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="55"/>
       <c r="F6" s="45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="56"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="E8" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1878,7 +1992,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1896,7 +2010,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -1954,7 +2068,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="54"/>
       <c r="C6" s="54"/>
@@ -1965,45 +2079,45 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2284,15 +2398,15 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC250FB9-90DD-47B4-83D2-014DDA78A0F9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2AE1A3-74BE-4713-8DFB-C5222E3FBD94}">
   <sheetPr>
     <tabColor theme="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,7 +2424,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -2368,124 +2482,110 @@
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="55"/>
       <c r="F6" s="45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="56"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>71</v>
+        <v>82</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="58" t="s">
-        <v>82</v>
+      <c r="A10" s="3"/>
+      <c r="B10" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="58" t="s">
-        <v>81</v>
+      <c r="A11" s="3"/>
+      <c r="B11" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="28"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="28"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
       <c r="D15" s="12"/>
@@ -2494,7 +2594,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
@@ -2503,60 +2603,58 @@
       <c r="F16" s="28"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="28"/>
+      <c r="D17" s="4"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="28"/>
+      <c r="A18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="27"/>
-      <c r="D19" s="4"/>
+      <c r="A19" s="3"/>
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="D20" s="4"/>
-      <c r="F20" s="7"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="D22" s="4"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="D23" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="22"/>
     </row>
     <row r="24" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
-      <c r="D24" s="17"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="28"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="18"/>
-      <c r="H24" s="10"/>
+      <c r="H24" s="22"/>
     </row>
     <row r="25" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="D25" s="17"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="20"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="28"/>
       <c r="G25" s="18"/>
       <c r="H25" s="22"/>
     </row>
@@ -2564,14 +2662,14 @@
       <c r="A26" s="11"/>
       <c r="D26" s="12"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="20"/>
+      <c r="F26" s="28"/>
       <c r="G26" s="18"/>
       <c r="H26" s="22"/>
     </row>
     <row r="27" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="14"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="23"/>
       <c r="F27" s="28"/>
       <c r="G27" s="18"/>
       <c r="H27" s="22"/>
@@ -2580,31 +2678,31 @@
       <c r="A28" s="11"/>
       <c r="D28" s="12"/>
       <c r="E28" s="14"/>
-      <c r="F28" s="28"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="18"/>
       <c r="H28" s="22"/>
     </row>
     <row r="29" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="D29" s="12"/>
-      <c r="E29" s="23"/>
+      <c r="E29" s="21"/>
       <c r="F29" s="28"/>
-      <c r="G29" s="18"/>
       <c r="H29" s="22"/>
     </row>
     <row r="30" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="D30" s="12"/>
       <c r="E30" s="14"/>
-      <c r="F30" s="24"/>
+      <c r="F30" s="28"/>
       <c r="G30" s="18"/>
       <c r="H30" s="22"/>
     </row>
     <row r="31" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="D31" s="12"/>
-      <c r="E31" s="21"/>
+      <c r="E31" s="19"/>
       <c r="F31" s="28"/>
+      <c r="G31" s="18"/>
       <c r="H31" s="22"/>
     </row>
     <row r="32" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -2618,7 +2716,7 @@
     <row r="33" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="D33" s="12"/>
-      <c r="E33" s="19"/>
+      <c r="E33" s="14"/>
       <c r="F33" s="28"/>
       <c r="G33" s="18"/>
       <c r="H33" s="22"/>
@@ -2626,17 +2724,17 @@
     <row r="34" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="D34" s="12"/>
-      <c r="E34" s="14"/>
+      <c r="E34" s="12"/>
       <c r="F34" s="28"/>
-      <c r="G34" s="18"/>
+      <c r="G34" s="12"/>
       <c r="H34" s="22"/>
     </row>
     <row r="35" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="D35" s="12"/>
-      <c r="E35" s="14"/>
+      <c r="E35" s="12"/>
       <c r="F35" s="28"/>
-      <c r="G35" s="18"/>
+      <c r="G35" s="12"/>
       <c r="H35" s="22"/>
     </row>
     <row r="36" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -2665,25 +2763,23 @@
     </row>
     <row r="39" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="14"/>
       <c r="F39" s="28"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="22"/>
     </row>
     <row r="40" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
+      <c r="E40" s="14"/>
       <c r="F40" s="28"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="22"/>
     </row>
     <row r="41" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="28"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
@@ -2691,48 +2787,34 @@
       <c r="E42" s="14"/>
       <c r="F42" s="28"/>
     </row>
-    <row r="43" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="28"/>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="27"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="29"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="27"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="8"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" s="27"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="32"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="14"/>
       <c r="F45" s="28"/>
-      <c r="G45" s="29"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" s="27"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="35"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="21"/>
       <c r="F46" s="8"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="28"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="27"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="8"/>
-      <c r="H48" s="28"/>
+      <c r="H46" s="28"/>
     </row>
   </sheetData>
   <dataConsolidate>
@@ -2748,4 +2830,2150 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC250FB9-90DD-47B4-83D2-014DDA78A0F9}">
+  <sheetPr>
+    <tabColor theme="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H46"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="33" customWidth="1"/>
+    <col min="6" max="6" width="99.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="41.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+    </row>
+    <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" s="11" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="56"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="57"/>
+      <c r="B7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="41"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="56"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="28"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="28"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="28"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="28"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="27"/>
+      <c r="D17" s="4"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="28"/>
+      <c r="H29" s="22"/>
+    </row>
+    <row r="30" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="22"/>
+    </row>
+    <row r="31" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="22"/>
+    </row>
+    <row r="36" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="22"/>
+    </row>
+    <row r="38" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="22"/>
+    </row>
+    <row r="39" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="28"/>
+    </row>
+    <row r="40" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="28"/>
+    </row>
+    <row r="41" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="28"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="27"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="29"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="27"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="28"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="27"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="8"/>
+      <c r="H46" s="28"/>
+    </row>
+  </sheetData>
+  <dataConsolidate>
+    <dataRefs count="1">
+      <dataRef ref="A2:H2" sheet="Status" r:id="rId1"/>
+    </dataRefs>
+  </dataConsolidate>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1BE4F3-9362-4ED1-9C83-0ABE86A3C90C}">
+  <sheetPr>
+    <tabColor theme="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H45"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="33" customWidth="1"/>
+    <col min="6" max="6" width="99.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="41.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+    </row>
+    <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" s="11" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="56"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="57"/>
+      <c r="B7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="41"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="56"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="28"/>
+    </row>
+    <row r="12" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="28"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="27"/>
+      <c r="D14" s="4"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="28"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="27"/>
+      <c r="D16" s="4"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="22"/>
+    </row>
+    <row r="23" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="28"/>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="22"/>
+    </row>
+    <row r="30" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="22"/>
+    </row>
+    <row r="31" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="22"/>
+    </row>
+    <row r="36" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="22"/>
+    </row>
+    <row r="38" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="28"/>
+    </row>
+    <row r="39" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="28"/>
+    </row>
+    <row r="40" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="28"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="27"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="29"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="27"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="8"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="28"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="27"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="8"/>
+      <c r="H45" s="28"/>
+    </row>
+  </sheetData>
+  <dataConsolidate>
+    <dataRefs count="1">
+      <dataRef ref="A2:H2" sheet="Status" r:id="rId1"/>
+    </dataRefs>
+  </dataConsolidate>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B46B5-CC98-4AFF-99BE-52A80444814C}">
+  <sheetPr>
+    <tabColor theme="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H48"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="33" customWidth="1"/>
+    <col min="6" max="6" width="99.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="41.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+    </row>
+    <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" s="11" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="56"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="57"/>
+      <c r="B7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="41"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="56"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="28"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="28"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="28"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="27"/>
+      <c r="D14" s="4"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="27"/>
+      <c r="D16" s="4"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="27"/>
+      <c r="D19" s="4"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="22"/>
+    </row>
+    <row r="30" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="22"/>
+    </row>
+    <row r="31" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="28"/>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="22"/>
+    </row>
+    <row r="36" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="22"/>
+    </row>
+    <row r="38" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="22"/>
+    </row>
+    <row r="39" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="22"/>
+    </row>
+    <row r="40" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="22"/>
+    </row>
+    <row r="41" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="28"/>
+    </row>
+    <row r="42" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="28"/>
+    </row>
+    <row r="43" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="28"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="27"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="29"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="27"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="28"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="27"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="8"/>
+      <c r="H48" s="28"/>
+    </row>
+  </sheetData>
+  <dataConsolidate>
+    <dataRefs count="1">
+      <dataRef ref="A2:H2" sheet="Status" r:id="rId1"/>
+    </dataRefs>
+  </dataConsolidate>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D2E8D7-01FA-43C5-BAE6-C758FD9BBBAB}">
+  <sheetPr>
+    <tabColor theme="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H48"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="33" customWidth="1"/>
+    <col min="6" max="6" width="99.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="41.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+    </row>
+    <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" s="11" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="56"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="57"/>
+      <c r="B7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="41"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="56"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="28"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="28"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="28"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="27"/>
+      <c r="D14" s="4"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="27"/>
+      <c r="D16" s="4"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="28"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="27"/>
+      <c r="D19" s="4"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="22"/>
+    </row>
+    <row r="30" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="22"/>
+    </row>
+    <row r="31" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="28"/>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="22"/>
+    </row>
+    <row r="36" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="22"/>
+    </row>
+    <row r="38" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="22"/>
+    </row>
+    <row r="39" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="22"/>
+    </row>
+    <row r="40" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="22"/>
+    </row>
+    <row r="41" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="28"/>
+    </row>
+    <row r="42" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="28"/>
+    </row>
+    <row r="43" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="28"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="27"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="29"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="27"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="28"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="27"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="8"/>
+      <c r="H48" s="28"/>
+    </row>
+  </sheetData>
+  <dataConsolidate>
+    <dataRefs count="1">
+      <dataRef ref="A2:H2" sheet="Status" r:id="rId1"/>
+    </dataRefs>
+  </dataConsolidate>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D4B318-96B3-4C12-9B6F-7FF26499C046}">
+  <sheetPr>
+    <tabColor theme="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H46"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="33" customWidth="1"/>
+    <col min="6" max="6" width="99.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="41.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+    </row>
+    <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" s="11" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="57"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="56"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="41"/>
+      <c r="E7" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="56"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="64" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="28"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="28"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="28"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="28"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="27"/>
+      <c r="D17" s="4"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="28"/>
+      <c r="H29" s="22"/>
+    </row>
+    <row r="30" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="22"/>
+    </row>
+    <row r="31" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="22"/>
+    </row>
+    <row r="36" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="22"/>
+    </row>
+    <row r="38" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="22"/>
+    </row>
+    <row r="39" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="28"/>
+    </row>
+    <row r="40" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="28"/>
+    </row>
+    <row r="41" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="28"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="27"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="29"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="27"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="28"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="27"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="8"/>
+      <c r="H46" s="28"/>
+    </row>
+  </sheetData>
+  <dataConsolidate>
+    <dataRefs count="1">
+      <dataRef ref="A2:H2" sheet="Status" r:id="rId1"/>
+    </dataRefs>
+  </dataConsolidate>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{9D558144-6A54-4FE2-A8B2-E47F0E0B0903}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Closed issues 11 and 17
</commit_message>
<xml_diff>
--- a/Draft Schema/Draft Weights and Condition Scores.xlsx
+++ b/Draft Schema/Draft Weights and Condition Scores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagaraja\Dropbox (Rezare Systems)\RezareProjects\MLA\ISC Animal Schema\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EDD229-7B8C-47CA-BACC-64F80D4B7D35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D237C162-FF0C-4EC7-B4BA-3BD4A6B2F862}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="749" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="icarEventCoreResource" sheetId="14" r:id="rId1"/>
@@ -42,7 +42,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="121">
   <si>
     <t>Entity</t>
   </si>
@@ -272,177 +274,178 @@
     </r>
   </si>
   <si>
+    <t>Body Site where the measurement was taken. Applicable for Fat Score</t>
+  </si>
+  <si>
+    <t>bodySite</t>
+  </si>
+  <si>
+    <t>assessor</t>
+  </si>
+  <si>
+    <t>Time in hours the animal has been off feed</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>iscEventCoreResource</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Usually measured in Millimeters. Applicable for Fat Score</t>
+  </si>
+  <si>
+    <t>traitLabel</t>
+  </si>
+  <si>
+    <t>iscScoreEventCore</t>
+  </si>
+  <si>
+    <t>iscScoreEventCore
+inherits allOf icarEventCoreResource</t>
+  </si>
+  <si>
+    <t>Y, default KGM</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>iscFatScore</t>
+  </si>
+  <si>
+    <t>iscConditionScore</t>
+  </si>
+  <si>
+    <t>iscFrameScore</t>
+  </si>
+  <si>
+    <t>iscMuscleScore</t>
+  </si>
+  <si>
+    <t>iscFatScore
+inherits allOf iscScoreEventCore</t>
+  </si>
+  <si>
+    <t>fatDepth</t>
+  </si>
+  <si>
+    <t>fatDepths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">array of boy sites and fat depth values </t>
+  </si>
+  <si>
+    <t>iscScoreReference</t>
+  </si>
+  <si>
+    <t>fatScoreReference</t>
+  </si>
+  <si>
+    <t>iscFrameScore
+inherits allOf iscScoreEventCore</t>
+  </si>
+  <si>
+    <t>frameScoreReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3, 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value of the fat score </t>
+  </si>
+  <si>
+    <t>iscMuscleScore
+inherits allOf iscScoreEventCore</t>
+  </si>
+  <si>
+    <t>muscleScoreReference</t>
+  </si>
+  <si>
+    <t>A, B, C, D, E</t>
+  </si>
+  <si>
+    <t>iscConditionScore
+inherits allOf iscScoreEventCore</t>
+  </si>
+  <si>
+    <t>conditionScoreReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, 2 </t>
+  </si>
+  <si>
+    <t>sting</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>referenceURL</t>
+  </si>
+  <si>
+    <t>nsw-beefcattle</t>
+  </si>
+  <si>
+    <t>https://www.dpi.nsw.gov.au/animals-and-livestock/beef-cattle/appraisal/publications/frame-scoring</t>
+  </si>
+  <si>
+    <t>Version reference of the particular scheme being followed for scoring</t>
+  </si>
+  <si>
+    <t>The scheme or scoring reference guideline being used</t>
+  </si>
+  <si>
+    <t>Ready links to documentation about the scoring scheme or reference being used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value of the muscle score . Muscle score measures the degree of muscularity of an animal and describes the shape of cattle independent of the influence of fatness. </t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>Event object for capturing Fat Score details</t>
+  </si>
+  <si>
+    <t>Event object for capturing Condition Score details</t>
+  </si>
+  <si>
+    <t>Event object for capturing Frame Score details</t>
+  </si>
+  <si>
+    <t>Event object for capturing Muscle Score details</t>
+  </si>
+  <si>
+    <t>Species for which the scoring scheme applies to</t>
+  </si>
+  <si>
+    <t>Country to which the scoring scheme appies to</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Value of the frame score. Frame score is a  convenient way to discuss and evaluate height is in units of 'frame score' based on the height over the hips at a given age</t>
+  </si>
+  <si>
+    <t>Value of the condition score . Body condition scoring is a visual assessment of the amount of fat and muscle covering the bones of a cow, regardless of body size</t>
+  </si>
+  <si>
     <t>Enumeration ( "Loadcell",
       "Girth",
       "Assessed",
       "WalkOver",
       "Predicted",
       "Imaged",
+"frontEndCorrelated",
       "GroupAverage"  )</t>
   </si>
   <si>
-    <t>Method by which the weight is observed. Includes loadcell (loadbars), girth (tape), assessed (visually), walk-over weighing,prediction, imaging (camera/IR), group average (pen weigh). Loadcell is the default if not specified.</t>
-  </si>
-  <si>
-    <t>Body Site where the measurement was taken. Applicable for Fat Score</t>
-  </si>
-  <si>
-    <t>bodySite</t>
-  </si>
-  <si>
-    <t>assessor</t>
-  </si>
-  <si>
-    <t>Time in hours the animal has been off feed</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>iscEventCoreResource</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Usually measured in Millimeters. Applicable for Fat Score</t>
-  </si>
-  <si>
-    <t>traitLabel</t>
-  </si>
-  <si>
-    <t>iscScoreEventCore</t>
-  </si>
-  <si>
-    <t>iscScoreEventCore
-inherits allOf icarEventCoreResource</t>
-  </si>
-  <si>
-    <t>Y, default KGM</t>
-  </si>
-  <si>
-    <t>double</t>
-  </si>
-  <si>
-    <t>iscFatScore</t>
-  </si>
-  <si>
-    <t>iscConditionScore</t>
-  </si>
-  <si>
-    <t>iscFrameScore</t>
-  </si>
-  <si>
-    <t>iscMuscleScore</t>
-  </si>
-  <si>
-    <t>iscFatScore
-inherits allOf iscScoreEventCore</t>
-  </si>
-  <si>
-    <t>fatDepth</t>
-  </si>
-  <si>
-    <t>fatDepths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">array of boy sites and fat depth values </t>
-  </si>
-  <si>
-    <t>iscScoreReference</t>
-  </si>
-  <si>
-    <t>fatScoreReference</t>
-  </si>
-  <si>
-    <t>iscFrameScore
-inherits allOf iscScoreEventCore</t>
-  </si>
-  <si>
-    <t>frameScoreReference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3, 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value of the fat score </t>
-  </si>
-  <si>
-    <t>iscMuscleScore
-inherits allOf iscScoreEventCore</t>
-  </si>
-  <si>
-    <t>muscleScoreReference</t>
-  </si>
-  <si>
-    <t>A, B, C, D, E</t>
-  </si>
-  <si>
-    <t>iscConditionScore
-inherits allOf iscScoreEventCore</t>
-  </si>
-  <si>
-    <t>conditionScoreReference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, 2 </t>
-  </si>
-  <si>
-    <t>sting</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>referenceURL</t>
-  </si>
-  <si>
-    <t>nsw-beefcattle</t>
-  </si>
-  <si>
-    <t>https://www.dpi.nsw.gov.au/animals-and-livestock/beef-cattle/appraisal/publications/frame-scoring</t>
-  </si>
-  <si>
-    <t>Version reference of the particular scheme being followed for scoring</t>
-  </si>
-  <si>
-    <t>The scheme or scoring reference guideline being used</t>
-  </si>
-  <si>
-    <t>Ready links to documentation about the scoring scheme or reference being used</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value of the muscle score . Muscle score measures the degree of muscularity of an animal and describes the shape of cattle independent of the influence of fatness. </t>
-  </si>
-  <si>
-    <t>species</t>
-  </si>
-  <si>
-    <t>Event object for capturing Fat Score details</t>
-  </si>
-  <si>
-    <t>Event object for capturing Condition Score details</t>
-  </si>
-  <si>
-    <t>Event object for capturing Frame Score details</t>
-  </si>
-  <si>
-    <t>Event object for capturing Muscle Score details</t>
-  </si>
-  <si>
-    <t>Species for which the scoring scheme applies to</t>
-  </si>
-  <si>
-    <t>Country to which the scoring scheme appies to</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>Value of the frame score. Frame score is a  convenient way to discuss and evaluate height is in units of 'frame score' based on the height over the hips at a given age</t>
-  </si>
-  <si>
-    <t>Value of the condition score . Body condition scoring is a visual assessment of the amount of fat and muscle covering the bones of a cow, regardless of body size</t>
+    <t xml:space="preserve">Method by which the weight is observed. Includes loadcell (loadbars), girth (tape), assessed (visually), walk-over weighing,prediction, imaging (camera/IR), front end correlated (The correlation of front-end body weight -partial body weight of the animal where only the front 2 legs are weighed to total body weight),  group average (pen weigh). </t>
   </si>
 </sst>
 </file>
@@ -745,6 +748,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -753,15 +765,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1113,7 +1116,7 @@
   </sheetPr>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -1131,29 +1134,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:8" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
@@ -1518,8 +1521,8 @@
   </sheetPr>
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,29 +1539,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
@@ -1616,10 +1619,10 @@
         <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>37</v>
@@ -1636,7 +1639,7 @@
         <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E8" s="38" t="s">
         <v>41</v>
@@ -1645,7 +1648,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
@@ -1653,10 +1656,10 @@
         <v>40</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1664,7 +1667,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>43</v>
@@ -1683,7 +1686,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>47</v>
@@ -1697,13 +1700,13 @@
         <v>63</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2009,29 +2012,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
@@ -2423,29 +2426,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="A1" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
@@ -2482,10 +2485,10 @@
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" s="54" t="s">
         <v>65</v>
@@ -2500,7 +2503,7 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
@@ -2515,53 +2518,53 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2841,7 +2844,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B12" sqref="B12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2858,29 +2861,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="A1" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
@@ -2917,13 +2920,13 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="55"/>
@@ -2935,15 +2938,15 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="57"/>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D7" s="41"/>
       <c r="E7" s="55"/>
       <c r="F7" s="45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G7" s="56"/>
     </row>
@@ -2956,45 +2959,56 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="62" t="s">
+      <c r="B10" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="59" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>60</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="62" t="s">
-        <v>81</v>
+      <c r="B11" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="59" t="s">
+        <v>79</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -3274,7 +3288,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B9" sqref="B9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3291,29 +3305,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="A1" s="62" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
@@ -3350,13 +3364,13 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="55"/>
@@ -3368,15 +3382,15 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="57"/>
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D7" s="41"/>
       <c r="E7" s="55"/>
       <c r="F7" s="45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G7" s="56"/>
     </row>
@@ -3388,10 +3402,21 @@
         <v>64</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3689,7 +3714,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B9" sqref="B9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3706,29 +3731,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="A1" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
@@ -3765,13 +3790,13 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="55"/>
@@ -3783,15 +3808,15 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="57"/>
       <c r="B7" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D7" s="41"/>
       <c r="E7" s="55"/>
       <c r="F7" s="45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G7" s="56"/>
     </row>
@@ -3803,10 +3828,21 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4119,7 +4155,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B9" sqref="B9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4136,29 +4172,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="A1" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
@@ -4195,13 +4231,13 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D6" s="41"/>
       <c r="E6" s="55"/>
@@ -4213,15 +4249,15 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="57"/>
       <c r="B7" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D7" s="41"/>
       <c r="E7" s="55"/>
       <c r="F7" s="45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G7" s="56"/>
     </row>
@@ -4233,10 +4269,21 @@
         <v>64</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4570,29 +4617,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="A1" s="62" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
@@ -4638,26 +4685,26 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="57" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D7" s="41"/>
       <c r="E7" s="55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F7" s="45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G7" s="56"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -4666,45 +4713,45 @@
         <v>1.3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="61" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="64" t="s">
-        <v>111</v>
       </c>
       <c r="C10" s="58" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="61" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="64" t="s">
-        <v>118</v>
       </c>
       <c r="C11" s="58" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>